<commit_message>
merged the statistics generating script into framework
</commit_message>
<xml_diff>
--- a/data/577 Projects/2013-2014/COCOMO Estimations.xlsx
+++ b/data/577 Projects/2013-2014/COCOMO Estimations.xlsx
@@ -531,20 +531,20 @@
   <dimension ref="A1:W7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+      <selection activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="34.28515625" customWidth="1"/>
     <col min="3" max="3" width="8.7109375" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="25.85546875" hidden="1" customWidth="1"/>
-    <col min="6" max="7" width="0" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="19.28515625" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="17.140625" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="25.5703125" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="15.28515625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="126.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.28515625" customWidth="1"/>
     <col min="12" max="12" width="22.5703125" customWidth="1"/>
     <col min="13" max="14" width="22" customWidth="1"/>
     <col min="15" max="15" width="21.7109375" customWidth="1"/>
@@ -818,11 +818,12 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
     <col min="5" max="5" width="15.140625" customWidth="1"/>
     <col min="6" max="6" width="22.5703125" customWidth="1"/>
     <col min="7" max="7" width="24.85546875" customWidth="1"/>

</xml_diff>

<commit_message>
added the data sheet for cocomo estimation from 2014-2015
</commit_message>
<xml_diff>
--- a/data/577 Projects/2013-2014/COCOMO Estimations.xlsx
+++ b/data/577 Projects/2013-2014/COCOMO Estimations.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11652" windowHeight="8616"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11655" windowHeight="8610"/>
   </bookViews>
   <sheets>
     <sheet name="Cocomo Effort Estimation" sheetId="1" r:id="rId1"/>
@@ -422,7 +422,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -648,23 +648,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -700,23 +683,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -898,33 +864,33 @@
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A63" sqref="A63:XFD63"/>
+      <selection pane="bottomLeft" activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="34.33203125" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="126.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.28515625" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="126.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="39" customWidth="1"/>
-    <col min="6" max="7" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.33203125" customWidth="1"/>
-    <col min="12" max="12" width="22.5546875" customWidth="1"/>
+    <col min="6" max="7" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.28515625" customWidth="1"/>
+    <col min="12" max="12" width="22.5703125" customWidth="1"/>
     <col min="13" max="14" width="22" customWidth="1"/>
-    <col min="15" max="15" width="21.6640625" customWidth="1"/>
-    <col min="16" max="16" width="24.88671875" customWidth="1"/>
-    <col min="17" max="17" width="19.33203125" customWidth="1"/>
-    <col min="19" max="19" width="18.6640625" customWidth="1"/>
-    <col min="20" max="20" width="18.88671875" customWidth="1"/>
-    <col min="21" max="21" width="24.109375" customWidth="1"/>
-    <col min="22" max="22" width="18.5546875" customWidth="1"/>
+    <col min="15" max="15" width="21.7109375" customWidth="1"/>
+    <col min="16" max="16" width="24.85546875" customWidth="1"/>
+    <col min="17" max="17" width="19.28515625" customWidth="1"/>
+    <col min="19" max="19" width="18.7109375" customWidth="1"/>
+    <col min="20" max="20" width="18.85546875" customWidth="1"/>
+    <col min="21" max="21" width="24.140625" customWidth="1"/>
+    <col min="22" max="22" width="18.5703125" customWidth="1"/>
     <col min="23" max="23" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -995,7 +961,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1012,7 +978,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1083,7 +1049,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E4" t="s">
         <v>31</v>
       </c>
@@ -1106,7 +1072,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
         <v>32</v>
       </c>
@@ -1129,7 +1095,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
         <v>33</v>
       </c>
@@ -1152,7 +1118,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
         <v>34</v>
       </c>
@@ -1175,7 +1141,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -1201,7 +1167,7 @@
       <c r="W16" s="4"/>
       <c r="X16" s="4"/>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>1</v>
       </c>
@@ -1239,7 +1205,7 @@
       <c r="W17" s="4"/>
       <c r="X17" s="4"/>
     </row>
-    <row r="18" spans="1:25" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:25" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="17"/>
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
@@ -1271,7 +1237,7 @@
       <c r="W18" s="17"/>
       <c r="X18" s="17"/>
     </row>
-    <row r="19" spans="1:25" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:25" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="17"/>
       <c r="B19" s="17"/>
       <c r="C19" s="17"/>
@@ -1303,7 +1269,7 @@
       <c r="W19" s="17"/>
       <c r="X19" s="17"/>
     </row>
-    <row r="20" spans="1:25" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:25" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="17"/>
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
@@ -1335,7 +1301,7 @@
       <c r="W20" s="17"/>
       <c r="X20" s="17"/>
     </row>
-    <row r="21" spans="1:25" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:25" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="17"/>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
@@ -1367,7 +1333,7 @@
       <c r="W21" s="17"/>
       <c r="X21" s="17"/>
     </row>
-    <row r="22" spans="1:25" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:25" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="17"/>
       <c r="B22" s="17"/>
       <c r="C22" s="17"/>
@@ -1393,7 +1359,7 @@
       <c r="W22" s="17"/>
       <c r="X22" s="17"/>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="16">
         <v>5</v>
       </c>
@@ -1461,7 +1427,7 @@
       <c r="X23" s="16"/>
       <c r="Y23" s="16"/>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
         <v>76</v>
       </c>
@@ -1484,7 +1450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E25" t="s">
         <v>75</v>
       </c>
@@ -1507,7 +1473,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E26" t="s">
         <v>74</v>
       </c>
@@ -1530,7 +1496,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E27" t="s">
         <v>73</v>
       </c>
@@ -1553,7 +1519,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -1593,7 +1559,7 @@
       <c r="W28" s="4"/>
       <c r="X28" s="4"/>
     </row>
-    <row r="29" spans="1:25" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:25" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="17"/>
       <c r="B29" s="17"/>
       <c r="C29" s="17"/>
@@ -1619,7 +1585,7 @@
       <c r="W29" s="17"/>
       <c r="X29" s="17"/>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>6</v>
       </c>
@@ -1685,7 +1651,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E31" t="s">
         <v>71</v>
       </c>
@@ -1708,7 +1674,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E32" t="s">
         <v>70</v>
       </c>
@@ -1731,7 +1697,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E33" t="s">
         <v>69</v>
       </c>
@@ -1754,7 +1720,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E34" t="s">
         <v>68</v>
       </c>
@@ -1777,7 +1743,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E35" t="s">
         <v>67</v>
       </c>
@@ -1800,7 +1766,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -1840,7 +1806,7 @@
       <c r="W36" s="4"/>
       <c r="X36" s="4"/>
     </row>
-    <row r="37" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="17"/>
@@ -1866,7 +1832,7 @@
       <c r="W37" s="4"/>
       <c r="X37" s="4"/>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>9</v>
       </c>
@@ -1899,7 +1865,7 @@
       <c r="W38" s="4"/>
       <c r="X38" s="4"/>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>14</v>
       </c>
@@ -1967,7 +1933,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E40" t="s">
         <v>64</v>
       </c>
@@ -1990,7 +1956,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E41" t="s">
         <v>63</v>
       </c>
@@ -2013,7 +1979,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E42" t="s">
         <v>62</v>
       </c>
@@ -2036,7 +2002,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="D43" s="4"/>
@@ -2075,7 +2041,7 @@
       <c r="W43" s="4"/>
       <c r="X43" s="4"/>
     </row>
-    <row r="44" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="17"/>
       <c r="B44" s="17"/>
       <c r="D44" s="17"/>
@@ -2100,7 +2066,7 @@
       <c r="W44" s="17"/>
       <c r="X44" s="17"/>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>3</v>
       </c>
@@ -2168,7 +2134,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E46" t="s">
         <v>59</v>
       </c>
@@ -2191,7 +2157,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E47" t="s">
         <v>58</v>
       </c>
@@ -2214,7 +2180,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E48" t="s">
         <v>57</v>
       </c>
@@ -2237,7 +2203,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
       <c r="B49" s="4"/>
       <c r="D49" s="4"/>
@@ -2276,7 +2242,7 @@
       <c r="W49" s="4"/>
       <c r="X49" s="4"/>
     </row>
-    <row r="50" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="17"/>
       <c r="B50" s="17"/>
       <c r="D50" s="17"/>
@@ -2301,7 +2267,7 @@
       <c r="W50" s="17"/>
       <c r="X50" s="17"/>
     </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>4</v>
       </c>
@@ -2318,7 +2284,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E52" t="s">
         <v>54</v>
       </c>
@@ -2326,7 +2292,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E53" t="s">
         <v>53</v>
       </c>
@@ -2334,7 +2300,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E54" t="s">
         <v>52</v>
       </c>
@@ -2342,7 +2308,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E55" t="s">
         <v>51</v>
       </c>
@@ -2350,7 +2316,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E56" t="s">
         <v>50</v>
       </c>
@@ -2361,7 +2327,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="57" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A57" s="4"/>
       <c r="B57" s="4"/>
       <c r="D57" s="4"/>
@@ -2392,7 +2358,7 @@
       <c r="W57" s="4"/>
       <c r="X57" s="4"/>
     </row>
-    <row r="58" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="17"/>
       <c r="B58" s="17"/>
       <c r="D58" s="17"/>
@@ -2417,7 +2383,7 @@
       <c r="W58" s="17"/>
       <c r="X58" s="17"/>
     </row>
-    <row r="59" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>6</v>
       </c>
@@ -2485,7 +2451,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="60" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
       <c r="D60" s="4"/>
@@ -2524,7 +2490,7 @@
       <c r="W60" s="4"/>
       <c r="X60" s="4"/>
     </row>
-    <row r="61" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="4"/>
       <c r="B61" s="4"/>
       <c r="D61" s="17"/>
@@ -2549,7 +2515,7 @@
       <c r="W61" s="4"/>
       <c r="X61" s="4"/>
     </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <v>12</v>
       </c>
@@ -2606,7 +2572,7 @@
       </c>
       <c r="X62" s="4"/>
     </row>
-    <row r="63" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="17"/>
       <c r="B63" s="17"/>
       <c r="E63" s="17"/>
@@ -2630,7 +2596,7 @@
       <c r="W63" s="17"/>
       <c r="X63" s="17"/>
     </row>
-    <row r="64" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>16</v>
       </c>
@@ -2698,7 +2664,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="65" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E65" t="s">
         <v>42</v>
       </c>
@@ -2721,7 +2687,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="66" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E66" t="s">
         <v>43</v>
       </c>
@@ -2744,7 +2710,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="67" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E67" t="s">
         <v>44</v>
       </c>
@@ -2767,7 +2733,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="68" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E68" t="s">
         <v>45</v>
       </c>
@@ -2790,7 +2756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E69" t="s">
         <v>46</v>
       </c>
@@ -2813,8 +2779,8 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="70" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="71" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A71" s="15">
         <v>2</v>
       </c>
@@ -2859,7 +2825,7 @@
       <c r="W71" s="16"/>
       <c r="X71" s="16"/>
     </row>
-    <row r="72" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E72" s="19" t="s">
         <v>98</v>
       </c>
@@ -2882,7 +2848,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="73" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E73" s="19"/>
       <c r="F73" s="19"/>
       <c r="G73" s="19"/>
@@ -2891,7 +2857,7 @@
       <c r="J73" s="19"/>
       <c r="K73" s="19"/>
     </row>
-    <row r="74" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A74" s="16">
         <v>7</v>
       </c>
@@ -2960,7 +2926,7 @@
       </c>
       <c r="X74" s="16"/>
     </row>
-    <row r="75" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E75" s="19" t="s">
         <v>101</v>
       </c>
@@ -2983,7 +2949,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="76" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E76" s="19" t="s">
         <v>102</v>
       </c>
@@ -3006,7 +2972,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="78" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A78" s="16">
         <v>8</v>
       </c>
@@ -3073,7 +3039,7 @@
       </c>
       <c r="X78" s="16"/>
     </row>
-    <row r="79" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E79" s="19" t="s">
         <v>104</v>
       </c>
@@ -3093,7 +3059,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="80" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E80" s="19" t="s">
         <v>105</v>
       </c>
@@ -3113,7 +3079,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="81" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E81" s="19" t="s">
         <v>106</v>
       </c>
@@ -3133,7 +3099,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="82" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E82" s="19" t="s">
         <v>107</v>
       </c>
@@ -3153,7 +3119,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="84" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A84" s="16">
         <v>10</v>
       </c>
@@ -3223,7 +3189,7 @@
       <c r="X84" s="16"/>
       <c r="Y84" s="16"/>
     </row>
-    <row r="85" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E85" s="19" t="s">
         <v>110</v>
       </c>
@@ -3246,7 +3212,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="86" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E86" s="19" t="s">
         <v>111</v>
       </c>
@@ -3269,7 +3235,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="87" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E87" s="19" t="s">
         <v>112</v>
       </c>
@@ -3292,7 +3258,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="88" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E88" s="19" t="s">
         <v>113</v>
       </c>
@@ -3315,7 +3281,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="89" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E89" s="19" t="s">
         <v>114</v>
       </c>
@@ -3338,7 +3304,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="91" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A91" s="16">
         <v>11</v>
       </c>
@@ -3407,7 +3373,7 @@
       </c>
       <c r="X91" s="16"/>
     </row>
-    <row r="92" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E92" s="19" t="s">
         <v>118</v>
       </c>
@@ -3430,7 +3396,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="93" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E93" s="19" t="s">
         <v>119</v>
       </c>
@@ -3453,7 +3419,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="94" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E94" s="19" t="s">
         <v>120</v>
       </c>
@@ -3476,7 +3442,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="95" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E95" s="19" t="s">
         <v>121</v>
       </c>
@@ -3499,7 +3465,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="96" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E96" s="19" t="s">
         <v>122</v>
       </c>
@@ -3522,7 +3488,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="97" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E97" s="19" t="s">
         <v>123</v>
       </c>
@@ -3545,7 +3511,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="99" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A99" s="16">
         <v>13</v>
       </c>
@@ -3615,7 +3581,7 @@
       <c r="X99" s="16"/>
       <c r="Y99" s="16"/>
     </row>
-    <row r="100" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E100" s="19" t="s">
         <v>126</v>
       </c>
@@ -3638,7 +3604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E101" s="19" t="s">
         <v>67</v>
       </c>
@@ -3661,7 +3627,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="102" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E102" s="19" t="s">
         <v>127</v>
       </c>
@@ -3684,7 +3650,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="103" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E103" s="19" t="s">
         <v>128</v>
       </c>
@@ -3707,7 +3673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A105" s="16">
         <v>15</v>
       </c>
@@ -3776,7 +3742,7 @@
       </c>
       <c r="X105" s="16"/>
     </row>
-    <row r="106" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E106" s="19" t="s">
         <v>67</v>
       </c>
@@ -3799,7 +3765,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="107" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E107" s="19" t="s">
         <v>130</v>
       </c>
@@ -3822,7 +3788,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="108" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E108" s="19" t="s">
         <v>132</v>
       </c>
@@ -3845,7 +3811,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="109" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E109" s="19" t="s">
         <v>131</v>
       </c>
@@ -3868,7 +3834,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="110" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E110" s="19" t="s">
         <v>133</v>
       </c>
@@ -3904,17 +3870,17 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="15.33203125" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" customWidth="1"/>
-    <col min="6" max="6" width="22.5546875" customWidth="1"/>
-    <col min="7" max="7" width="24.88671875" customWidth="1"/>
-    <col min="8" max="8" width="18.88671875" customWidth="1"/>
-    <col min="9" max="9" width="19.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" customWidth="1"/>
+    <col min="7" max="7" width="24.85546875" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -3949,7 +3915,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -3975,7 +3941,7 @@
         <v>3113</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4011,7 +3977,7 @@
         <v>1592</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
fixed the 9 data points for evaluation
</commit_message>
<xml_diff>
--- a/data/577 Projects/2013-2014/COCOMO Estimations.xlsx
+++ b/data/577 Projects/2013-2014/COCOMO Estimations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11652" windowHeight="8616"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11655" windowHeight="8610"/>
   </bookViews>
   <sheets>
     <sheet name="Cocomo Effort Estimation" sheetId="1" r:id="rId1"/>
@@ -865,38 +865,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y122"/>
+  <dimension ref="A1:Y123"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="D29" sqref="D29"/>
+      <selection pane="bottomLeft" activeCell="F124" sqref="F124"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="34.33203125" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="126.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.28515625" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="62.5703125" customWidth="1"/>
     <col min="5" max="5" width="39" customWidth="1"/>
-    <col min="6" max="7" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.33203125" customWidth="1"/>
-    <col min="12" max="12" width="22.5546875" customWidth="1"/>
+    <col min="6" max="7" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.28515625" customWidth="1"/>
+    <col min="12" max="12" width="22.5703125" customWidth="1"/>
     <col min="13" max="14" width="22" customWidth="1"/>
-    <col min="15" max="15" width="21.6640625" customWidth="1"/>
-    <col min="16" max="16" width="24.88671875" customWidth="1"/>
-    <col min="17" max="17" width="19.33203125" customWidth="1"/>
-    <col min="19" max="19" width="18.6640625" customWidth="1"/>
-    <col min="20" max="20" width="18.88671875" customWidth="1"/>
-    <col min="21" max="21" width="24.109375" customWidth="1"/>
-    <col min="22" max="22" width="18.5546875" customWidth="1"/>
+    <col min="15" max="15" width="21.7109375" customWidth="1"/>
+    <col min="16" max="16" width="24.85546875" customWidth="1"/>
+    <col min="17" max="17" width="19.28515625" customWidth="1"/>
+    <col min="19" max="19" width="18.7109375" customWidth="1"/>
+    <col min="20" max="20" width="18.85546875" customWidth="1"/>
+    <col min="21" max="21" width="24.140625" customWidth="1"/>
+    <col min="22" max="22" width="18.5703125" customWidth="1"/>
     <col min="23" max="23" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -967,7 +967,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -984,7 +984,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1055,7 +1055,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E4" t="s">
         <v>31</v>
       </c>
@@ -1082,7 +1082,7 @@
         <v>1088.32</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
         <v>32</v>
       </c>
@@ -1105,7 +1105,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
         <v>33</v>
       </c>
@@ -1128,7 +1128,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
         <v>34</v>
       </c>
@@ -1151,7 +1151,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -1177,7 +1177,7 @@
       <c r="W16" s="4"/>
       <c r="X16" s="4"/>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>1</v>
       </c>
@@ -1217,7 +1217,7 @@
       <c r="W17" s="4"/>
       <c r="X17" s="4"/>
     </row>
-    <row r="18" spans="1:25" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:25" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="17"/>
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
@@ -1249,7 +1249,7 @@
       <c r="W18" s="17"/>
       <c r="X18" s="17"/>
     </row>
-    <row r="19" spans="1:25" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:25" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="17"/>
       <c r="B19" s="17"/>
       <c r="C19" s="17"/>
@@ -1281,7 +1281,7 @@
       <c r="W19" s="17"/>
       <c r="X19" s="17"/>
     </row>
-    <row r="20" spans="1:25" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:25" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="17"/>
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
@@ -1313,7 +1313,7 @@
       <c r="W20" s="17"/>
       <c r="X20" s="17"/>
     </row>
-    <row r="21" spans="1:25" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:25" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="17"/>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
@@ -1345,7 +1345,7 @@
       <c r="W21" s="17"/>
       <c r="X21" s="17"/>
     </row>
-    <row r="22" spans="1:25" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:25" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="17"/>
       <c r="B22" s="17"/>
       <c r="C22" s="17"/>
@@ -1376,7 +1376,7 @@
       <c r="W22" s="17"/>
       <c r="X22" s="17"/>
     </row>
-    <row r="23" spans="1:25" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:25" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="17"/>
       <c r="B23" s="17"/>
       <c r="C23" s="17"/>
@@ -1402,7 +1402,7 @@
       <c r="W23" s="17"/>
       <c r="X23" s="17"/>
     </row>
-    <row r="24" spans="1:25" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:25" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="17"/>
       <c r="B24" s="17"/>
       <c r="C24" s="17"/>
@@ -1428,7 +1428,7 @@
       <c r="W24" s="17"/>
       <c r="X24" s="17"/>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="16">
         <v>5</v>
       </c>
@@ -1496,7 +1496,7 @@
       <c r="X25" s="16"/>
       <c r="Y25" s="16"/>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E26" t="s">
         <v>76</v>
       </c>
@@ -1523,7 +1523,7 @@
         <v>577.6</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E27" t="s">
         <v>75</v>
       </c>
@@ -1546,7 +1546,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E28" t="s">
         <v>74</v>
       </c>
@@ -1569,7 +1569,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E29" t="s">
         <v>73</v>
       </c>
@@ -1592,7 +1592,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -1632,7 +1632,7 @@
       <c r="W30" s="4"/>
       <c r="X30" s="4"/>
     </row>
-    <row r="31" spans="1:25" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:25" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="17"/>
       <c r="B31" s="17"/>
       <c r="C31" s="17"/>
@@ -1663,7 +1663,7 @@
       <c r="W31" s="17"/>
       <c r="X31" s="17"/>
     </row>
-    <row r="32" spans="1:25" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:25" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="17"/>
       <c r="B32" s="17"/>
       <c r="C32" s="17"/>
@@ -1689,7 +1689,7 @@
       <c r="W32" s="17"/>
       <c r="X32" s="17"/>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>6</v>
       </c>
@@ -1755,7 +1755,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E34" t="s">
         <v>71</v>
       </c>
@@ -1782,7 +1782,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E35" t="s">
         <v>70</v>
       </c>
@@ -1805,7 +1805,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E36" t="s">
         <v>69</v>
       </c>
@@ -1828,7 +1828,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E37" t="s">
         <v>68</v>
       </c>
@@ -1851,7 +1851,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E38" t="s">
         <v>67</v>
       </c>
@@ -1874,7 +1874,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -1914,7 +1914,7 @@
       <c r="W39" s="4"/>
       <c r="X39" s="4"/>
     </row>
-    <row r="40" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="17"/>
@@ -1945,7 +1945,7 @@
       <c r="W40" s="4"/>
       <c r="X40" s="4"/>
     </row>
-    <row r="41" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="17"/>
@@ -1971,7 +1971,7 @@
       <c r="W41" s="4"/>
       <c r="X41" s="4"/>
     </row>
-    <row r="42" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="17"/>
@@ -1997,7 +1997,7 @@
       <c r="W42" s="4"/>
       <c r="X42" s="4"/>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>9</v>
       </c>
@@ -2030,7 +2030,7 @@
       <c r="W43" s="4"/>
       <c r="X43" s="4"/>
     </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>14</v>
       </c>
@@ -2098,7 +2098,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E45" t="s">
         <v>64</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E46" t="s">
         <v>63</v>
       </c>
@@ -2148,7 +2148,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E47" t="s">
         <v>62</v>
       </c>
@@ -2171,7 +2171,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="D48" s="4"/>
@@ -2210,7 +2210,7 @@
       <c r="W48" s="4"/>
       <c r="X48" s="4"/>
     </row>
-    <row r="49" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="17"/>
       <c r="B49" s="17"/>
       <c r="D49" s="17"/>
@@ -2240,7 +2240,7 @@
       <c r="W49" s="17"/>
       <c r="X49" s="17"/>
     </row>
-    <row r="50" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="17"/>
       <c r="B50" s="17"/>
       <c r="D50" s="17"/>
@@ -2265,7 +2265,7 @@
       <c r="W50" s="17"/>
       <c r="X50" s="17"/>
     </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>3</v>
       </c>
@@ -2333,7 +2333,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E52" t="s">
         <v>59</v>
       </c>
@@ -2360,7 +2360,7 @@
         <v>541.12</v>
       </c>
     </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E53" t="s">
         <v>58</v>
       </c>
@@ -2383,7 +2383,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E54" t="s">
         <v>57</v>
       </c>
@@ -2406,7 +2406,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
       <c r="B55" s="4"/>
       <c r="D55" s="4"/>
@@ -2445,7 +2445,7 @@
       <c r="W55" s="4"/>
       <c r="X55" s="4"/>
     </row>
-    <row r="56" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="17"/>
       <c r="B56" s="17"/>
       <c r="D56" s="17"/>
@@ -2475,7 +2475,7 @@
       <c r="W56" s="17"/>
       <c r="X56" s="17"/>
     </row>
-    <row r="57" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="17"/>
       <c r="B57" s="17"/>
       <c r="D57" s="17"/>
@@ -2500,7 +2500,7 @@
       <c r="W57" s="17"/>
       <c r="X57" s="17"/>
     </row>
-    <row r="58" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>4</v>
       </c>
@@ -2520,7 +2520,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="59" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E59" t="s">
         <v>54</v>
       </c>
@@ -2528,7 +2528,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="60" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E60" t="s">
         <v>53</v>
       </c>
@@ -2536,7 +2536,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="61" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E61" t="s">
         <v>52</v>
       </c>
@@ -2544,7 +2544,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E62" t="s">
         <v>51</v>
       </c>
@@ -2552,7 +2552,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="63" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E63" t="s">
         <v>50</v>
       </c>
@@ -2563,7 +2563,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="64" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
       <c r="B64" s="4"/>
       <c r="D64" s="4"/>
@@ -2594,7 +2594,7 @@
       <c r="W64" s="4"/>
       <c r="X64" s="4"/>
     </row>
-    <row r="65" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="17"/>
       <c r="B65" s="17"/>
       <c r="D65" s="17"/>
@@ -2624,7 +2624,7 @@
       <c r="W65" s="17"/>
       <c r="X65" s="17"/>
     </row>
-    <row r="66" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="17"/>
       <c r="B66" s="17"/>
       <c r="D66" s="17"/>
@@ -2649,7 +2649,7 @@
       <c r="W66" s="17"/>
       <c r="X66" s="17"/>
     </row>
-    <row r="67" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="17"/>
       <c r="B67" s="17"/>
       <c r="D67" s="17"/>
@@ -2674,7 +2674,7 @@
       <c r="W67" s="17"/>
       <c r="X67" s="17"/>
     </row>
-    <row r="68" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>6</v>
       </c>
@@ -2742,7 +2742,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="69" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A69" s="4"/>
       <c r="B69" s="4"/>
       <c r="D69" s="4"/>
@@ -2784,7 +2784,7 @@
       <c r="W69" s="4"/>
       <c r="X69" s="4"/>
     </row>
-    <row r="70" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
       <c r="D70" s="17"/>
@@ -2813,7 +2813,7 @@
       <c r="W70" s="4"/>
       <c r="X70" s="4"/>
     </row>
-    <row r="71" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
       <c r="D71" s="17"/>
@@ -2838,7 +2838,7 @@
       <c r="W71" s="4"/>
       <c r="X71" s="4"/>
     </row>
-    <row r="72" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
         <v>12</v>
       </c>
@@ -2895,7 +2895,7 @@
       </c>
       <c r="X72" s="4"/>
     </row>
-    <row r="73" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="17"/>
       <c r="B73" s="17"/>
       <c r="E73" s="17"/>
@@ -2919,7 +2919,7 @@
       <c r="W73" s="17"/>
       <c r="X73" s="17"/>
     </row>
-    <row r="74" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="17"/>
       <c r="B74" s="17"/>
       <c r="E74" s="17"/>
@@ -2946,7 +2946,7 @@
       <c r="W74" s="17"/>
       <c r="X74" s="17"/>
     </row>
-    <row r="75" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>16</v>
       </c>
@@ -3014,7 +3014,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="76" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E76" t="s">
         <v>42</v>
       </c>
@@ -3041,7 +3041,7 @@
         <v>1506.32</v>
       </c>
     </row>
-    <row r="77" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E77" t="s">
         <v>43</v>
       </c>
@@ -3064,7 +3064,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="78" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E78" t="s">
         <v>44</v>
       </c>
@@ -3087,7 +3087,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="79" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E79" t="s">
         <v>45</v>
       </c>
@@ -3110,7 +3110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E80" t="s">
         <v>46</v>
       </c>
@@ -3133,8 +3133,8 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="81" spans="1:25" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="82" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:25" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="82" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A82" s="15">
         <v>2</v>
       </c>
@@ -3181,7 +3181,7 @@
       <c r="W82" s="16"/>
       <c r="X82" s="16"/>
     </row>
-    <row r="83" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E83" s="19" t="s">
         <v>98</v>
       </c>
@@ -3204,7 +3204,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="84" spans="1:25" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:25" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E84" s="19" t="s">
         <v>135</v>
       </c>
@@ -3218,7 +3218,7 @@
       <c r="J84" s="19"/>
       <c r="K84" s="19"/>
     </row>
-    <row r="85" spans="1:25" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:25" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E85" s="19"/>
       <c r="F85" s="19"/>
       <c r="G85" s="19"/>
@@ -3227,7 +3227,7 @@
       <c r="J85" s="19"/>
       <c r="K85" s="19"/>
     </row>
-    <row r="86" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A86" s="16">
         <v>7</v>
       </c>
@@ -3296,7 +3296,7 @@
       </c>
       <c r="X86" s="16"/>
     </row>
-    <row r="87" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E87" s="19" t="s">
         <v>101</v>
       </c>
@@ -3323,7 +3323,7 @@
         <v>1045.76</v>
       </c>
     </row>
-    <row r="88" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E88" s="19" t="s">
         <v>102</v>
       </c>
@@ -3346,7 +3346,13 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="90" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="F89">
+        <f>SUM(F86:F88)</f>
+        <v>3795</v>
+      </c>
+    </row>
+    <row r="90" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A90" s="16">
         <v>8</v>
       </c>
@@ -3413,7 +3419,7 @@
       </c>
       <c r="X90" s="16"/>
     </row>
-    <row r="91" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E91" s="19" t="s">
         <v>104</v>
       </c>
@@ -3437,7 +3443,7 @@
         <v>1810.32</v>
       </c>
     </row>
-    <row r="92" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E92" s="19" t="s">
         <v>105</v>
       </c>
@@ -3457,7 +3463,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="93" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E93" s="19" t="s">
         <v>106</v>
       </c>
@@ -3477,7 +3483,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="94" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E94" s="19" t="s">
         <v>107</v>
       </c>
@@ -3497,7 +3503,13 @@
         <v>277</v>
       </c>
     </row>
-    <row r="96" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="F95">
+        <f>SUM(F90:F94)</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="96" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A96" s="16">
         <v>10</v>
       </c>
@@ -3567,7 +3579,7 @@
       <c r="X96" s="16"/>
       <c r="Y96" s="16"/>
     </row>
-    <row r="97" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E97" s="19" t="s">
         <v>110</v>
       </c>
@@ -3594,7 +3606,7 @@
         <v>1393.84</v>
       </c>
     </row>
-    <row r="98" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E98" s="19" t="s">
         <v>111</v>
       </c>
@@ -3617,7 +3629,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="99" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E99" s="19" t="s">
         <v>112</v>
       </c>
@@ -3640,7 +3652,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="100" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E100" s="19" t="s">
         <v>113</v>
       </c>
@@ -3663,7 +3675,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="101" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E101" s="19" t="s">
         <v>114</v>
       </c>
@@ -3686,7 +3698,13 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="103" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="F102">
+        <f>SUM(F96:F101)</f>
+        <v>7776</v>
+      </c>
+    </row>
+    <row r="103" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A103" s="16">
         <v>11</v>
       </c>
@@ -3755,7 +3773,7 @@
       </c>
       <c r="X103" s="16"/>
     </row>
-    <row r="104" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E104" s="19" t="s">
         <v>118</v>
       </c>
@@ -3782,7 +3800,7 @@
         <v>1092.8800000000001</v>
       </c>
     </row>
-    <row r="105" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E105" s="19" t="s">
         <v>119</v>
       </c>
@@ -3805,7 +3823,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="106" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E106" s="19" t="s">
         <v>120</v>
       </c>
@@ -3828,7 +3846,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="107" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E107" s="19" t="s">
         <v>121</v>
       </c>
@@ -3851,7 +3869,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="108" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E108" s="19" t="s">
         <v>122</v>
       </c>
@@ -3874,7 +3892,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="109" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E109" s="19" t="s">
         <v>123</v>
       </c>
@@ -3897,7 +3915,13 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="111" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="F110">
+        <f>SUM(F103:F109)</f>
+        <v>4095</v>
+      </c>
+    </row>
+    <row r="111" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A111" s="16">
         <v>13</v>
       </c>
@@ -3967,7 +3991,7 @@
       <c r="X111" s="16"/>
       <c r="Y111" s="16"/>
     </row>
-    <row r="112" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E112" s="19" t="s">
         <v>126</v>
       </c>
@@ -3994,7 +4018,7 @@
         <v>1741.92</v>
       </c>
     </row>
-    <row r="113" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E113" s="19" t="s">
         <v>67</v>
       </c>
@@ -4017,7 +4041,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="114" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E114" s="19" t="s">
         <v>127</v>
       </c>
@@ -4040,7 +4064,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="115" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E115" s="19" t="s">
         <v>128</v>
       </c>
@@ -4063,7 +4087,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="F116">
+        <f>SUM(F111:F115)</f>
+        <v>3507</v>
+      </c>
+    </row>
+    <row r="117" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A117" s="16">
         <v>15</v>
       </c>
@@ -4132,7 +4162,7 @@
       </c>
       <c r="X117" s="16"/>
     </row>
-    <row r="118" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E118" s="19" t="s">
         <v>67</v>
       </c>
@@ -4159,7 +4189,7 @@
         <v>1295.04</v>
       </c>
     </row>
-    <row r="119" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E119" s="19" t="s">
         <v>130</v>
       </c>
@@ -4182,7 +4212,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="120" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E120" s="19" t="s">
         <v>132</v>
       </c>
@@ -4205,7 +4235,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="121" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E121" s="19" t="s">
         <v>131</v>
       </c>
@@ -4228,7 +4258,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="122" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E122" s="19" t="s">
         <v>133</v>
       </c>
@@ -4249,6 +4279,12 @@
       </c>
       <c r="K122" s="19">
         <v>0.2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="F123">
+        <f>SUM(F117:F122)</f>
+        <v>3600</v>
       </c>
     </row>
   </sheetData>
@@ -4264,17 +4300,17 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="15.33203125" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" customWidth="1"/>
-    <col min="6" max="6" width="22.5546875" customWidth="1"/>
-    <col min="7" max="7" width="24.88671875" customWidth="1"/>
-    <col min="8" max="8" width="18.88671875" customWidth="1"/>
-    <col min="9" max="9" width="19.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" customWidth="1"/>
+    <col min="7" max="7" width="24.85546875" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -4309,7 +4345,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -4335,7 +4371,7 @@
         <v>3113</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4371,7 +4407,7 @@
         <v>1592</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
         <v>39</v>
       </c>

</xml_diff>